<commit_message>
flipbooks preguntas abiertas 3/10
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/31_formato_cargue_preguntas_abiertas.xlsx
+++ b/assets/formatos_cargue/31_formato_cargue_preguntas_abiertas.xlsx
@@ -19,33 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Cód. tema</t>
   </si>
   <si>
-    <t>l1-u01</t>
-  </si>
-  <si>
     <t>Texto pregunta</t>
   </si>
   <si>
-    <t>¿De qué tamaño es el sol?</t>
-  </si>
-  <si>
-    <t>¿A qué distancia está la luna?</t>
-  </si>
-  <si>
-    <t>¿Qué opina de la NASA?</t>
-  </si>
-  <si>
-    <t>¿Cuál cree es es el papel de los bomberos?</t>
-  </si>
-  <si>
-    <t>tema no</t>
-  </si>
-  <si>
-    <t>la pregunta</t>
+    <t>en7-u01</t>
+  </si>
+  <si>
+    <t>¿Lorem ipsum dolor sit amet, consectetur adipiscing elit. In mi ante, ultricies eu massa vitae, maximus faucibus nisl.?</t>
+  </si>
+  <si>
+    <t>¿Nulla efficitur purus a risus gravida, quis mattis urna semper?</t>
+  </si>
+  <si>
+    <t>¿Aenean bibendum ante vitae mi ultrices, nec dictum nibh vulputate. Maecenas fermentum blandit nibh, a cursus risus lobortis eu?</t>
+  </si>
+  <si>
+    <t>¿In gravida cursus quam at aliquam. Sed erat nunc, accumsan a gravida ac, maximus ut est?</t>
+  </si>
+  <si>
+    <t>en7-u02</t>
   </si>
 </sst>
 </file>
@@ -421,7 +418,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +440,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -455,7 +452,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -463,7 +460,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -471,7 +468,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -479,24 +476,14 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Flipbooks en formato de clase dinamica version 1
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/31_formato_cargue_preguntas_abiertas.xlsx
+++ b/assets/formatos_cargue/31_formato_cargue_preguntas_abiertas.xlsx
@@ -27,9 +27,6 @@
     <t>Texto pregunta</t>
   </si>
   <si>
-    <t>en7-u01</t>
-  </si>
-  <si>
     <t>¿Lorem ipsum dolor sit amet, consectetur adipiscing elit. In mi ante, ultricies eu massa vitae, maximus faucibus nisl.?</t>
   </si>
   <si>
@@ -42,7 +39,10 @@
     <t>¿In gravida cursus quam at aliquam. Sed erat nunc, accumsan a gravida ac, maximus ut est?</t>
   </si>
   <si>
-    <t>en7-u02</t>
+    <t>en5-u01</t>
+  </si>
+  <si>
+    <t>en5-u02</t>
   </si>
 </sst>
 </file>
@@ -452,18 +452,18 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -471,7 +471,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -479,7 +479,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>